<commit_message>
#77 #76 #75 #74
</commit_message>
<xml_diff>
--- a/Solution/ProjetoX/teste.xlsx
+++ b/Solution/ProjetoX/teste.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Registros" r:id="rId3" sheetId="1"/>
+    <sheet name="Relatorios" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Nº do contrato</t>
   </si>
@@ -41,7 +41,7 @@
     <t>R$ 1.090,00</t>
   </si>
   <si>
-    <t>-R$ 90,00</t>
+    <t>R$ 90,00</t>
   </si>
   <si>
     <t>2</t>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>-R$ 1.000,00</t>
   </si>
 </sst>
 </file>
@@ -110,32 +113,32 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="30"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="30"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="30"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="30"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -193,7 +196,7 @@
     <col min="2" max="2" width="28.96875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="27.09765625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.2109375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.2265625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.41015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -261,7 +264,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>